<commit_message>
horas extra october system
</commit_message>
<xml_diff>
--- a/2022/7.julio2022.xlsx
+++ b/2022/7.julio2022.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>SISTEMA INTEGRADO DE GESTION</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Alistamiento y cambio de IP , integración de antena y sensor de fondo</t>
+  </si>
+  <si>
+    <t>20/07/2022</t>
+  </si>
+  <si>
+    <t>Soporte en Campo Azor-2</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-240A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -286,6 +292,12 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -864,7 +876,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1094,85 +1106,19 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1187,6 +1133,81 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1208,14 +1229,8 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1602,8 +1617,8 @@
   </sheetPr>
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
@@ -1619,100 +1634,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A1" s="87"/>
-      <c r="B1" s="88"/>
-      <c r="C1" s="104" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="98" t="s">
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="99"/>
+      <c r="L1" s="108"/>
     </row>
     <row r="2" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A2" s="89"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="108"/>
     </row>
     <row r="3" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="98" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="99"/>
+      <c r="L3" s="108"/>
       <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="96" t="s">
+      <c r="A4" s="98"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="110"/>
       <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:25" ht="11.25" customHeight="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="102" t="s">
+      <c r="A5" s="98"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="103"/>
+      <c r="L5" s="112"/>
     </row>
     <row r="6" spans="1:25" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
     </row>
     <row r="7" spans="1:25" ht="6" customHeight="1" thickBot="1">
       <c r="A7" s="7"/>
@@ -1786,54 +1801,54 @@
       <c r="L10" s="67"/>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110" t="s">
+      <c r="C11" s="90"/>
+      <c r="D11" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="110" t="s">
+      <c r="E11" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="108" t="s">
+      <c r="F11" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="108" t="s">
+      <c r="G11" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="110" t="s">
+      <c r="H11" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="110" t="s">
+      <c r="I11" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="110" t="s">
+      <c r="J11" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="108" t="s">
+      <c r="K11" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="112" t="s">
+      <c r="L11" s="119" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A12" s="94"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="113"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="120"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1849,22 +1864,22 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" ht="22.5" customHeight="1">
-      <c r="A13" s="95"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="113"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="120"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2049,10 +2064,10 @@
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="126" t="s">
+      <c r="J18" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="125" t="s">
+      <c r="K18" s="87" t="s">
         <v>39</v>
       </c>
       <c r="L18" s="25"/>
@@ -2082,7 +2097,7 @@
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
-      <c r="F19" s="127">
+      <c r="F19" s="89">
         <v>8</v>
       </c>
       <c r="G19" s="32"/>
@@ -2091,7 +2106,7 @@
       <c r="J19" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="125" t="s">
+      <c r="K19" s="87" t="s">
         <v>39</v>
       </c>
       <c r="L19" s="25"/>
@@ -2110,17 +2125,29 @@
       <c r="Y19" s="2"/>
     </row>
     <row r="20" spans="1:25" ht="20.149999999999999" customHeight="1">
-      <c r="A20" s="47"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="42">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C20" s="43">
+        <v>0.25</v>
+      </c>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="F20" s="32">
+        <v>8</v>
+      </c>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
+      <c r="J20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="L20" s="25"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2146,7 +2173,7 @@
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
-      <c r="J21" s="24"/>
+      <c r="J21" s="128"/>
       <c r="K21" s="24"/>
       <c r="L21" s="25"/>
       <c r="M21" s="2"/>
@@ -2623,11 +2650,11 @@
       <c r="Y38" s="2"/>
     </row>
     <row r="39" spans="1:25" ht="20.149999999999999" customHeight="1" thickBot="1">
-      <c r="A39" s="115" t="s">
+      <c r="A39" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="116"/>
-      <c r="C39" s="117"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="95"/>
       <c r="D39" s="38">
         <f>SUM(D15:D38)</f>
         <v>8</v>
@@ -2638,7 +2665,7 @@
       </c>
       <c r="F39" s="40">
         <f>SUM(F14:F38)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G39" s="40">
         <f t="shared" ref="G39:H39" si="0">SUM(G14:G38)</f>
@@ -2669,12 +2696,12 @@
     <row r="41" spans="1:25" ht="24" customHeight="1">
       <c r="D41" s="6"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="114"/>
-      <c r="G41" s="114"/>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="92"/>
       <c r="L41" s="17"/>
     </row>
     <row r="42" spans="1:25" ht="13">
@@ -2693,11 +2720,11 @@
     </row>
     <row r="43" spans="1:25" ht="59.25" customHeight="1">
       <c r="A43" s="5"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
       <c r="D43" s="18"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="92"/>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
@@ -2707,11 +2734,11 @@
       <c r="M43" s="3"/>
     </row>
     <row r="44" spans="1:25" ht="13">
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
@@ -2795,13 +2822,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="F41:K41"/>
     <mergeCell ref="A1:B6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C4:J6"/>
@@ -2818,6 +2838,13 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="F41:K41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2848,23 +2875,23 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" thickBot="1"/>
     <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="120"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="3" spans="1:6" ht="14">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="126" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="69"/>
@@ -2872,9 +2899,9 @@
       <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6" ht="28">
-      <c r="A4" s="122"/>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
+      <c r="A4" s="125"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
       <c r="D4" s="71" t="s">
         <v>28</v>
       </c>

</xml_diff>